<commit_message>
Finish user story 4 and 5 Remove calling methods in gedcom.py
</commit_message>
<xml_diff>
--- a/Team_M2JC_Report.xlsx
+++ b/Team_M2JC_Report.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maryam\Downloads\555-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lanslot\OneDrive\课程相关\17Fall\CS 555\Project\555\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="D1F89168FB057B755066A2A655A317B81BD9ED13" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{747ED1DC-9AC9-4D83-BC9F-CC130E4DAB43}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="463" windowWidth="28800" windowHeight="16423" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="168">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -501,12 +502,6 @@
   </si>
   <si>
     <t>MY</t>
-  </si>
-  <si>
-    <t>LIU</t>
-  </si>
-  <si>
-    <t>TIU</t>
   </si>
   <si>
     <t>cs</t>
@@ -580,7 +575,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -589,35 +584,37 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Cambria"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -637,6 +634,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -729,24 +742,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -783,84 +787,95 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="65">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -878,7 +893,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1015,7 +1030,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1948,121 +1963,121 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.06640625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.84375" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.84375" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.4609375" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4609375" style="28" customWidth="1"/>
-    <col min="6" max="16384" width="11.07421875" style="28"/>
+    <col min="1" max="1" width="7.86328125" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.86328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.46484375" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="11.06640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="E4" s="28" t="s">
+      <c r="B6" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="D9" s="26" t="s">
+    <row r="9" spans="1:8" ht="16.3" x14ac:dyDescent="0.4">
+      <c r="D9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="25">
         <v>555</v>
       </c>
-      <c r="G9" s="29"/>
-    </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-    </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="G12" s="30"/>
-      <c r="H12" s="31"/>
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.3" x14ac:dyDescent="0.4">
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.3" x14ac:dyDescent="0.4">
+      <c r="G11" s="27"/>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.3" x14ac:dyDescent="0.4">
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -2088,66 +2103,66 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.06640625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="9.4609375" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.86328125" style="5"/>
+    <col min="2" max="2" width="9.46484375" customWidth="1"/>
+    <col min="3" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.86328125" customWidth="1"/>
+    <col min="6" max="6" width="12.46484375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2155,114 +2170,114 @@
       <c r="A15" t="s">
         <v>131</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="8">
         <v>41065</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="9">
         <v>24</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="9">
         <v>0</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="8">
         <v>41078</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="9">
         <v>18</v>
       </c>
       <c r="D16">
         <f>C15-C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="9">
         <v>250</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="9">
         <v>120</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="7">
         <f>(E16-E15)/F16*60</f>
         <v>125.00000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="8">
         <v>41092</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="9">
         <v>12</v>
       </c>
       <c r="D17">
         <f t="shared" ref="D17:D19" si="0">C16-C17</f>
         <v>6</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="9">
         <v>480</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="10">
         <v>135</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="7">
         <f t="shared" ref="G17:G19" si="1">(E17-E16)/F17*60</f>
         <v>102.22222222222223</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="8">
         <v>41106</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="9">
         <v>6</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="9">
         <v>740</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="10">
         <v>160</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="7">
         <f t="shared" si="1"/>
         <v>97.5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="8">
         <v>41120</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="9">
         <v>0</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="9">
         <v>1100</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="10">
         <v>145</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="7">
         <f t="shared" si="1"/>
         <v>148.9655172413793</v>
       </c>
@@ -2282,38 +2297,38 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.06640625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.86328125" style="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.46484375" customWidth="1"/>
+    <col min="4" max="4" width="7.1328125" customWidth="1"/>
+    <col min="5" max="5" width="6.86328125" customWidth="1"/>
+    <col min="6" max="6" width="12.46484375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>41535</v>
       </c>
       <c r="B2">
@@ -2339,281 +2354,281 @@
       <selection activeCell="H10" sqref="E10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.06640625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.15234375" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.69140625" customWidth="1"/>
+    <col min="2" max="2" width="32.1328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.84375" style="6"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.86328125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="14">
         <v>75</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="14">
         <v>60</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="20"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="14">
+        <v>75</v>
+      </c>
+      <c r="F3" s="14">
+        <v>60</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="14">
+        <v>75</v>
+      </c>
+      <c r="F4" s="14">
+        <v>60</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="14">
+        <v>75</v>
+      </c>
+      <c r="F5" s="14">
+        <v>60</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="14">
+        <v>75</v>
+      </c>
+      <c r="F6" s="14">
+        <v>60</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="14">
+        <v>75</v>
+      </c>
+      <c r="F7" s="14">
+        <v>60</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E8" s="14">
         <v>75</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F8" s="14">
         <v>60</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="17" t="s">
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E9" s="14">
         <v>75</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F9" s="14">
         <v>60</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="20"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="17">
-        <v>75</v>
-      </c>
-      <c r="F5" s="17">
-        <v>60</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="20"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="17">
-        <v>75</v>
-      </c>
-      <c r="F6" s="17">
-        <v>60</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="17">
-        <v>75</v>
-      </c>
-      <c r="F7" s="17">
-        <v>60</v>
-      </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="20"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="17">
-        <v>75</v>
-      </c>
-      <c r="F8" s="17">
-        <v>60</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="20"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="17">
-        <v>75</v>
-      </c>
-      <c r="F9" s="17">
-        <v>60</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="20"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <f>SUM(E2:E9)</f>
         <v>600</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="21">
         <f>SUM(F2:F9)</f>
         <v>480</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <f>SUM(G2:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <f>SUM(H2:H9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="21"/>
-      <c r="I15" s="7"/>
+      <c r="B15" s="18"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2632,206 +2647,206 @@
       <selection activeCell="E10" sqref="E10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.06640625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.4609375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.46484375" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="D2" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="D3" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="D8" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="D9" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <f>SUM(E2:E9)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="21">
         <f>SUM(F2:F9)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <f>SUM(G2:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <f>SUM(H2:H9)</f>
         <v>0</v>
       </c>
@@ -2851,168 +2866,168 @@
       <selection activeCell="E10" sqref="E10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="17"/>
-    <col min="2" max="2" width="26.4609375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.84375" style="17"/>
+    <col min="1" max="1" width="10.86328125" style="14"/>
+    <col min="2" max="2" width="26.46484375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.86328125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>169</v>
+      <c r="D2" s="14" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>169</v>
+      <c r="D3" s="14" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="D8" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>169</v>
+      <c r="D9" s="14" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <f>SUM(E2:E9)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="21">
         <f>SUM(F2:F9)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <f>SUM(G2:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <f>SUM(H2:H9)</f>
         <v>0</v>
       </c>
@@ -3031,168 +3046,168 @@
       <selection activeCell="E10" sqref="E10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="17"/>
-    <col min="2" max="2" width="26" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.84375" style="17"/>
+    <col min="1" max="1" width="10.86328125" style="14"/>
+    <col min="2" max="2" width="26" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.86328125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>169</v>
+      <c r="D2" s="14" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>169</v>
+      <c r="D3" s="14" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="D8" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>169</v>
+      <c r="D9" s="14" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <f>SUM(E2:E9)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="21">
         <f>SUM(F2:F9)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <f>SUM(G2:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <f>SUM(H2:H9)</f>
         <v>0</v>
       </c>
@@ -3208,434 +3223,436 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.06640625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.06640625" style="31"/>
+    <col min="2" max="2" width="28.1328125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.46484375" style="33" customWidth="1"/>
+    <col min="4" max="16384" width="11.06640625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="30" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="31" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="31" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="31" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" t="s">
-        <v>149</v>
-      </c>
-    </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="D9" t="s">
-        <v>149</v>
+      <c r="D9" s="31" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="32" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="32" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="32" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.3">
+      <c r="A14" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="32" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="32" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="32" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="32" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="32" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="32" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="32" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="32" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="32" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="32" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="32" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="32" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="32" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="32" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="32" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="32" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C34" s="10"/>
+      <c r="C34" s="32"/>
     </row>
     <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C35" s="10"/>
+      <c r="C35" s="32"/>
     </row>
     <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C36" s="10"/>
+      <c r="C36" s="32"/>
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C37" s="10"/>
+      <c r="C37" s="32"/>
     </row>
     <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C38" s="10"/>
+      <c r="C38" s="32"/>
     </row>
     <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C39" s="10"/>
+      <c r="C39" s="32"/>
     </row>
     <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C40" s="10"/>
+      <c r="C40" s="32"/>
     </row>
     <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C41" s="10"/>
+      <c r="C41" s="32"/>
     </row>
     <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C42" s="10"/>
+      <c r="C42" s="32"/>
     </row>
     <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="C43" s="10"/>
+      <c r="C43" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>